<commit_message>
fix lab_1. Math error
</commit_message>
<xml_diff>
--- a/Lab_1/bin/Debug/net5.0/Graphs.xlsx
+++ b/Lab_1/bin/Debug/net5.0/Graphs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\ReposProject\NumericalMethod_RUDN\Lab_1\bin\Debug\net5.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\C#\NumericalMethod_RUDN\Lab_1\bin\Debug\net5.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8D59996-8841-4640-A710-AE5F4443BDA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DD54E7-BEE9-4016-BDFB-A1570AE7493B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{B87D9D6C-919A-4869-B71D-CF2C2FCA4C8B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B87D9D6C-919A-4869-B71D-CF2C2FCA4C8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -110,7 +110,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1104,304 +1104,304 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>1.0157400000000001</c:v>
+                  <c:v>1.0137223</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.04443</c:v>
+                  <c:v>1.0442442000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0813600000000001</c:v>
+                  <c:v>1.0814561</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1246799999999999</c:v>
+                  <c:v>1.1245552999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1732</c:v>
+                  <c:v>1.1727818000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.22603</c:v>
+                  <c:v>1.2253936999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.28237</c:v>
+                  <c:v>1.2816738999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.34155</c:v>
+                  <c:v>1.3409297</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4029400000000001</c:v>
+                  <c:v>1.4025027000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.4659199999999999</c:v>
+                  <c:v>1.4657292</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.5299199999999999</c:v>
+                  <c:v>1.5299995</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.5944</c:v>
+                  <c:v>1.5947182</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.65882</c:v>
+                  <c:v>1.6593149</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.7226600000000001</c:v>
+                  <c:v>1.7232529999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.7854099999999999</c:v>
+                  <c:v>1.7859905</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.84657</c:v>
+                  <c:v>1.8470397999999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.90567</c:v>
+                  <c:v>1.9059280999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.9622599999999999</c:v>
+                  <c:v>1.9622066</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.0158900000000002</c:v>
+                  <c:v>2.0154589999999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.0661299999999998</c:v>
+                  <c:v>2.0652688000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.11259</c:v>
+                  <c:v>2.1112690000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.15489</c:v>
+                  <c:v>2.1531083999999998</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.1926600000000001</c:v>
+                  <c:v>2.1904604000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2255699999999998</c:v>
+                  <c:v>2.223023</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.25332</c:v>
+                  <c:v>2.2505220000000001</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.2756099999999999</c:v>
+                  <c:v>2.2726950000000001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.2922099999999999</c:v>
+                  <c:v>2.2893178000000001</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.3028900000000001</c:v>
+                  <c:v>2.3001862000000002</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.3074499999999998</c:v>
+                  <c:v>2.3051192999999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.3057400000000001</c:v>
+                  <c:v>2.3039608</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.2976200000000002</c:v>
+                  <c:v>2.2965797999999999</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.28301</c:v>
+                  <c:v>2.2828693000000002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.2618399999999999</c:v>
+                  <c:v>2.2627467999999999</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.23407</c:v>
+                  <c:v>2.2361537999999999</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.1997300000000002</c:v>
+                  <c:v>2.2030568000000001</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.15883</c:v>
+                  <c:v>2.1634395</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.1114700000000002</c:v>
+                  <c:v>2.1173294</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.05776</c:v>
+                  <c:v>2.0647597000000002</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.9978199999999999</c:v>
+                  <c:v>2.0057947999999999</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.93184</c:v>
+                  <c:v>1.9405227</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.8600099999999999</c:v>
+                  <c:v>1.8690439999999999</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.7826</c:v>
+                  <c:v>1.7915182999999999</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.6998599999999999</c:v>
+                  <c:v>1.7080964999999999</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.61209</c:v>
+                  <c:v>1.6189642</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.51962</c:v>
+                  <c:v>1.5243316</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.4227799999999999</c:v>
+                  <c:v>1.4244169</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.3220000000000001</c:v>
+                  <c:v>1.3195110000000001</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.21766</c:v>
+                  <c:v>1.2098819999999999</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.1101799999999999</c:v>
+                  <c:v>1.0958376000000001</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1</c:v>
+                  <c:v>0.97770999999999997</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.88761000000000001</c:v>
+                  <c:v>0.85585580000000006</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.77344999999999997</c:v>
+                  <c:v>0.7306359</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.65805000000000002</c:v>
+                  <c:v>0.60249560000000002</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.54191999999999996</c:v>
+                  <c:v>0.47184512000000001</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.42554999999999998</c:v>
+                  <c:v>0.33913865999999998</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.30947999999999998</c:v>
+                  <c:v>0.20485485</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.19422</c:v>
+                  <c:v>6.9475174000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>8.0329999999999999E-2</c:v>
+                  <c:v>-6.6429790000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-3.1669999999999997E-2</c:v>
+                  <c:v>-0.20232964000000001</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>-0.14126</c:v>
+                  <c:v>-0.33764810000000001</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>-0.24790000000000001</c:v>
+                  <c:v>-0.47178456000000002</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>-0.35110000000000002</c:v>
+                  <c:v>-0.60411389999999998</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>-0.45034000000000002</c:v>
+                  <c:v>-0.73400710000000002</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>-0.54510999999999998</c:v>
+                  <c:v>-0.86074894999999996</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>-0.63495000000000001</c:v>
+                  <c:v>-0.98366189999999998</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>-0.71938000000000002</c:v>
+                  <c:v>-1.1020234</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>-0.79796999999999996</c:v>
+                  <c:v>-1.2150862</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>-0.87029999999999996</c:v>
+                  <c:v>-1.3220955000000001</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>-0.93594999999999995</c:v>
+                  <c:v>-1.4222212000000001</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>-0.99455000000000005</c:v>
+                  <c:v>-1.5146603999999999</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>-1.0457700000000001</c:v>
+                  <c:v>-1.5985685999999999</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>-1.08927</c:v>
+                  <c:v>-1.6730765000000001</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>-1.1247799999999999</c:v>
+                  <c:v>-1.7373000000000001</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>-1.1520300000000001</c:v>
+                  <c:v>-1.7903007</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>-1.1708000000000001</c:v>
+                  <c:v>-1.8311474000000001</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>-1.18092</c:v>
+                  <c:v>-1.8588731999999999</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>-1.18221</c:v>
+                  <c:v>-1.8724871000000001</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>-1.17458</c:v>
+                  <c:v>-1.8709735000000001</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>-1.15794</c:v>
+                  <c:v>-1.8532883</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>-1.13226</c:v>
+                  <c:v>-1.8183727000000001</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>-1.09754</c:v>
+                  <c:v>-1.7651365000000001</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>-1.05382</c:v>
+                  <c:v>-1.6924665000000001</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>-1.00118</c:v>
+                  <c:v>-1.5992252</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>-0.93972</c:v>
+                  <c:v>-1.4842303999999999</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>-0.86963000000000001</c:v>
+                  <c:v>-1.3463323</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>-0.79110000000000003</c:v>
+                  <c:v>-1.1843036</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>-0.70435000000000003</c:v>
+                  <c:v>-0.99690920000000005</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>-0.60967000000000005</c:v>
+                  <c:v>-0.78288939999999996</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>-0.50736000000000003</c:v>
+                  <c:v>-0.54096040000000001</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>-0.39774999999999999</c:v>
+                  <c:v>-0.26976805999999998</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>-0.28125</c:v>
+                  <c:v>3.1934104999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>-0.15826999999999999</c:v>
+                  <c:v>0.36554414000000002</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>-2.9239999999999999E-2</c:v>
+                  <c:v>0.73244363000000001</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.10535</c:v>
+                  <c:v>1.1340386</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.24503</c:v>
+                  <c:v>1.5718319999999999</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.38923000000000002</c:v>
+                  <c:v>2.0471393999999998</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.53739999999999999</c:v>
+                  <c:v>2.5615070000000002</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.68898999999999999</c:v>
+                  <c:v>3.1164382000000002</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.84338999999999997</c:v>
+                  <c:v>3.7134610000000001</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1.0000100000000001</c:v>
+                  <c:v>4.3542337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2229,9 +2229,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2269,7 +2269,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2375,7 +2375,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2528,7 +2528,7 @@
   <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,7 +2564,7 @@
         <v>6.2829999999999997E-2</v>
       </c>
       <c r="D2">
-        <v>1.0157400000000001</v>
+        <v>1.0137223</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2578,7 +2578,7 @@
         <v>0.12565999999999999</v>
       </c>
       <c r="D3">
-        <v>1.04443</v>
+        <v>1.0442442000000001</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2592,7 +2592,7 @@
         <v>0.1885</v>
       </c>
       <c r="D4">
-        <v>1.0813600000000001</v>
+        <v>1.0814561</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2606,7 +2606,7 @@
         <v>0.25133</v>
       </c>
       <c r="D5">
-        <v>1.1246799999999999</v>
+        <v>1.1245552999999999</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2620,7 +2620,7 @@
         <v>0.31415999999999999</v>
       </c>
       <c r="D6">
-        <v>1.1732</v>
+        <v>1.1727818000000001</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2634,7 +2634,7 @@
         <v>0.37698999999999999</v>
       </c>
       <c r="D7">
-        <v>1.22603</v>
+        <v>1.2253936999999999</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2648,7 +2648,7 @@
         <v>0.43981999999999999</v>
       </c>
       <c r="D8">
-        <v>1.28237</v>
+        <v>1.2816738999999999</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2662,7 +2662,7 @@
         <v>0.50265000000000004</v>
       </c>
       <c r="D9">
-        <v>1.34155</v>
+        <v>1.3409297</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2676,7 +2676,7 @@
         <v>0.56549000000000005</v>
       </c>
       <c r="D10">
-        <v>1.4029400000000001</v>
+        <v>1.4025027000000001</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2690,7 +2690,7 @@
         <v>0.62831999999999999</v>
       </c>
       <c r="D11">
-        <v>1.4659199999999999</v>
+        <v>1.4657292</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2704,7 +2704,7 @@
         <v>0.69115000000000004</v>
       </c>
       <c r="D12">
-        <v>1.5299199999999999</v>
+        <v>1.5299995</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2718,7 +2718,7 @@
         <v>0.75397999999999998</v>
       </c>
       <c r="D13">
-        <v>1.5944</v>
+        <v>1.5947182</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2732,7 +2732,7 @@
         <v>0.81681000000000004</v>
       </c>
       <c r="D14">
-        <v>1.65882</v>
+        <v>1.6593149</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2746,7 +2746,7 @@
         <v>0.87965000000000004</v>
       </c>
       <c r="D15">
-        <v>1.7226600000000001</v>
+        <v>1.7232529999999999</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2760,7 +2760,7 @@
         <v>0.94247999999999998</v>
       </c>
       <c r="D16">
-        <v>1.7854099999999999</v>
+        <v>1.7859905</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2774,7 +2774,7 @@
         <v>1.0053099999999999</v>
       </c>
       <c r="D17">
-        <v>1.84657</v>
+        <v>1.8470397999999999</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2788,7 +2788,7 @@
         <v>1.0681400000000001</v>
       </c>
       <c r="D18">
-        <v>1.90567</v>
+        <v>1.9059280999999999</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2802,7 +2802,7 @@
         <v>1.13097</v>
       </c>
       <c r="D19">
-        <v>1.9622599999999999</v>
+        <v>1.9622066</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2816,7 +2816,7 @@
         <v>1.19381</v>
       </c>
       <c r="D20">
-        <v>2.0158900000000002</v>
+        <v>2.0154589999999999</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2830,7 +2830,7 @@
         <v>1.25664</v>
       </c>
       <c r="D21">
-        <v>2.0661299999999998</v>
+        <v>2.0652688000000001</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2844,7 +2844,7 @@
         <v>1.3194699999999999</v>
       </c>
       <c r="D22">
-        <v>2.11259</v>
+        <v>2.1112690000000001</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2858,7 +2858,7 @@
         <v>1.3823000000000001</v>
       </c>
       <c r="D23">
-        <v>2.15489</v>
+        <v>2.1531083999999998</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2872,7 +2872,7 @@
         <v>1.44513</v>
       </c>
       <c r="D24">
-        <v>2.1926600000000001</v>
+        <v>2.1904604000000001</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2886,7 +2886,7 @@
         <v>1.50796</v>
       </c>
       <c r="D25">
-        <v>2.2255699999999998</v>
+        <v>2.223023</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2900,7 +2900,7 @@
         <v>1.5708</v>
       </c>
       <c r="D26">
-        <v>2.25332</v>
+        <v>2.2505220000000001</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2914,7 +2914,7 @@
         <v>1.6336299999999999</v>
       </c>
       <c r="D27">
-        <v>2.2756099999999999</v>
+        <v>2.2726950000000001</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2928,7 +2928,7 @@
         <v>1.6964600000000001</v>
       </c>
       <c r="D28">
-        <v>2.2922099999999999</v>
+        <v>2.2893178000000001</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2942,7 +2942,7 @@
         <v>1.75929</v>
       </c>
       <c r="D29">
-        <v>2.3028900000000001</v>
+        <v>2.3001862000000002</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2956,7 +2956,7 @@
         <v>1.82212</v>
       </c>
       <c r="D30">
-        <v>2.3074499999999998</v>
+        <v>2.3051192999999999</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2970,7 +2970,7 @@
         <v>1.88496</v>
       </c>
       <c r="D31">
-        <v>2.3057400000000001</v>
+        <v>2.3039608</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2984,7 +2984,7 @@
         <v>1.9477899999999999</v>
       </c>
       <c r="D32">
-        <v>2.2976200000000002</v>
+        <v>2.2965797999999999</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2998,7 +2998,7 @@
         <v>2.0106199999999999</v>
       </c>
       <c r="D33">
-        <v>2.28301</v>
+        <v>2.2828693000000002</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3012,7 +3012,7 @@
         <v>2.0734499999999998</v>
       </c>
       <c r="D34">
-        <v>2.2618399999999999</v>
+        <v>2.2627467999999999</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3026,7 +3026,7 @@
         <v>2.1362800000000002</v>
       </c>
       <c r="D35">
-        <v>2.23407</v>
+        <v>2.2361537999999999</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3040,7 +3040,7 @@
         <v>2.1991100000000001</v>
       </c>
       <c r="D36">
-        <v>2.1997300000000002</v>
+        <v>2.2030568000000001</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3054,7 +3054,7 @@
         <v>2.2619500000000001</v>
       </c>
       <c r="D37">
-        <v>2.15883</v>
+        <v>2.1634395</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3068,7 +3068,7 @@
         <v>2.3247800000000001</v>
       </c>
       <c r="D38">
-        <v>2.1114700000000002</v>
+        <v>2.1173294</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3082,7 +3082,7 @@
         <v>2.38761</v>
       </c>
       <c r="D39">
-        <v>2.05776</v>
+        <v>2.0647597000000002</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3096,7 +3096,7 @@
         <v>2.45044</v>
       </c>
       <c r="D40">
-        <v>1.9978199999999999</v>
+        <v>2.0057947999999999</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3110,7 +3110,7 @@
         <v>2.5132699999999999</v>
       </c>
       <c r="D41">
-        <v>1.93184</v>
+        <v>1.9405227</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3124,7 +3124,7 @@
         <v>2.5761099999999999</v>
       </c>
       <c r="D42">
-        <v>1.8600099999999999</v>
+        <v>1.8690439999999999</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3138,7 +3138,7 @@
         <v>2.6389399999999998</v>
       </c>
       <c r="D43">
-        <v>1.7826</v>
+        <v>1.7915182999999999</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3152,7 +3152,7 @@
         <v>2.7017699999999998</v>
       </c>
       <c r="D44">
-        <v>1.6998599999999999</v>
+        <v>1.7080964999999999</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3166,7 +3166,7 @@
         <v>2.7646000000000002</v>
       </c>
       <c r="D45">
-        <v>1.61209</v>
+        <v>1.6189642</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3180,7 +3180,7 @@
         <v>2.8274300000000001</v>
       </c>
       <c r="D46">
-        <v>1.51962</v>
+        <v>1.5243316</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3194,7 +3194,7 @@
         <v>2.8902700000000001</v>
       </c>
       <c r="D47">
-        <v>1.4227799999999999</v>
+        <v>1.4244169</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3208,7 +3208,7 @@
         <v>2.9531000000000001</v>
       </c>
       <c r="D48">
-        <v>1.3220000000000001</v>
+        <v>1.3195110000000001</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3222,7 +3222,7 @@
         <v>3.01593</v>
       </c>
       <c r="D49">
-        <v>1.21766</v>
+        <v>1.2098819999999999</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3236,7 +3236,7 @@
         <v>3.0787599999999999</v>
       </c>
       <c r="D50">
-        <v>1.1101799999999999</v>
+        <v>1.0958376000000001</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3250,7 +3250,7 @@
         <v>3.1415899999999999</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>0.97770999999999997</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3264,7 +3264,7 @@
         <v>3.2044199999999998</v>
       </c>
       <c r="D52">
-        <v>0.88761000000000001</v>
+        <v>0.85585580000000006</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3278,7 +3278,7 @@
         <v>3.2672599999999998</v>
       </c>
       <c r="D53">
-        <v>0.77344999999999997</v>
+        <v>0.7306359</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3292,7 +3292,7 @@
         <v>3.3300900000000002</v>
       </c>
       <c r="D54">
-        <v>0.65805000000000002</v>
+        <v>0.60249560000000002</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3306,7 +3306,7 @@
         <v>3.3929200000000002</v>
       </c>
       <c r="D55">
-        <v>0.54191999999999996</v>
+        <v>0.47184512000000001</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3320,7 +3320,7 @@
         <v>3.4557500000000001</v>
       </c>
       <c r="D56">
-        <v>0.42554999999999998</v>
+        <v>0.33913865999999998</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3334,7 +3334,7 @@
         <v>3.51858</v>
       </c>
       <c r="D57">
-        <v>0.30947999999999998</v>
+        <v>0.20485485</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3348,7 +3348,7 @@
         <v>3.58142</v>
       </c>
       <c r="D58">
-        <v>0.19422</v>
+        <v>6.9475174000000001E-2</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3362,7 +3362,7 @@
         <v>3.64425</v>
       </c>
       <c r="D59">
-        <v>8.0329999999999999E-2</v>
+        <v>-6.6429790000000002E-2</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3376,7 +3376,7 @@
         <v>3.7070799999999999</v>
       </c>
       <c r="D60">
-        <v>-3.1669999999999997E-2</v>
+        <v>-0.20232964000000001</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3390,7 +3390,7 @@
         <v>3.7699099999999999</v>
       </c>
       <c r="D61">
-        <v>-0.14126</v>
+        <v>-0.33764810000000001</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3404,7 +3404,7 @@
         <v>3.8327399999999998</v>
       </c>
       <c r="D62">
-        <v>-0.24790000000000001</v>
+        <v>-0.47178456000000002</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3418,7 +3418,7 @@
         <v>3.8955700000000002</v>
       </c>
       <c r="D63">
-        <v>-0.35110000000000002</v>
+        <v>-0.60411389999999998</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3432,7 +3432,7 @@
         <v>3.9584100000000002</v>
       </c>
       <c r="D64">
-        <v>-0.45034000000000002</v>
+        <v>-0.73400710000000002</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3446,7 +3446,7 @@
         <v>4.0212399999999997</v>
       </c>
       <c r="D65">
-        <v>-0.54510999999999998</v>
+        <v>-0.86074894999999996</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3460,7 +3460,7 @@
         <v>4.0840699999999996</v>
       </c>
       <c r="D66">
-        <v>-0.63495000000000001</v>
+        <v>-0.98366189999999998</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3474,7 +3474,7 @@
         <v>4.1468999999999996</v>
       </c>
       <c r="D67">
-        <v>-0.71938000000000002</v>
+        <v>-1.1020234</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3488,7 +3488,7 @@
         <v>4.2097300000000004</v>
       </c>
       <c r="D68">
-        <v>-0.79796999999999996</v>
+        <v>-1.2150862</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3502,7 +3502,7 @@
         <v>4.27257</v>
       </c>
       <c r="D69">
-        <v>-0.87029999999999996</v>
+        <v>-1.3220955000000001</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3516,7 +3516,7 @@
         <v>4.3353999999999999</v>
       </c>
       <c r="D70">
-        <v>-0.93594999999999995</v>
+        <v>-1.4222212000000001</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3530,7 +3530,7 @@
         <v>4.3982299999999999</v>
       </c>
       <c r="D71">
-        <v>-0.99455000000000005</v>
+        <v>-1.5146603999999999</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3544,7 +3544,7 @@
         <v>4.4610599999999998</v>
       </c>
       <c r="D72">
-        <v>-1.0457700000000001</v>
+        <v>-1.5985685999999999</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3558,7 +3558,7 @@
         <v>4.5238899999999997</v>
       </c>
       <c r="D73">
-        <v>-1.08927</v>
+        <v>-1.6730765000000001</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3572,7 +3572,7 @@
         <v>4.5867300000000002</v>
       </c>
       <c r="D74">
-        <v>-1.1247799999999999</v>
+        <v>-1.7373000000000001</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3586,7 +3586,7 @@
         <v>4.6495600000000001</v>
       </c>
       <c r="D75">
-        <v>-1.1520300000000001</v>
+        <v>-1.7903007</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3600,7 +3600,7 @@
         <v>4.7123900000000001</v>
       </c>
       <c r="D76">
-        <v>-1.1708000000000001</v>
+        <v>-1.8311474000000001</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3614,7 +3614,7 @@
         <v>4.77522</v>
       </c>
       <c r="D77">
-        <v>-1.18092</v>
+        <v>-1.8588731999999999</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -3628,7 +3628,7 @@
         <v>4.83805</v>
       </c>
       <c r="D78">
-        <v>-1.18221</v>
+        <v>-1.8724871000000001</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -3642,7 +3642,7 @@
         <v>4.9008799999999999</v>
       </c>
       <c r="D79">
-        <v>-1.17458</v>
+        <v>-1.8709735000000001</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -3656,7 +3656,7 @@
         <v>4.9637200000000004</v>
       </c>
       <c r="D80">
-        <v>-1.15794</v>
+        <v>-1.8532883</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -3670,7 +3670,7 @@
         <v>5.0265500000000003</v>
       </c>
       <c r="D81">
-        <v>-1.13226</v>
+        <v>-1.8183727000000001</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -3684,7 +3684,7 @@
         <v>5.0893800000000002</v>
       </c>
       <c r="D82">
-        <v>-1.09754</v>
+        <v>-1.7651365000000001</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -3698,7 +3698,7 @@
         <v>5.1522100000000002</v>
       </c>
       <c r="D83">
-        <v>-1.05382</v>
+        <v>-1.6924665000000001</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -3712,7 +3712,7 @@
         <v>5.2150400000000001</v>
       </c>
       <c r="D84">
-        <v>-1.00118</v>
+        <v>-1.5992252</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -3726,7 +3726,7 @@
         <v>5.2778799999999997</v>
       </c>
       <c r="D85">
-        <v>-0.93972</v>
+        <v>-1.4842303999999999</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -3740,7 +3740,7 @@
         <v>5.3407099999999996</v>
       </c>
       <c r="D86">
-        <v>-0.86963000000000001</v>
+        <v>-1.3463323</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -3754,7 +3754,7 @@
         <v>5.4035399999999996</v>
       </c>
       <c r="D87">
-        <v>-0.79110000000000003</v>
+        <v>-1.1843036</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -3768,7 +3768,7 @@
         <v>5.4663700000000004</v>
       </c>
       <c r="D88">
-        <v>-0.70435000000000003</v>
+        <v>-0.99690920000000005</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -3782,7 +3782,7 @@
         <v>5.5292000000000003</v>
       </c>
       <c r="D89">
-        <v>-0.60967000000000005</v>
+        <v>-0.78288939999999996</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -3796,7 +3796,7 @@
         <v>5.5920300000000003</v>
       </c>
       <c r="D90">
-        <v>-0.50736000000000003</v>
+        <v>-0.54096040000000001</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -3810,7 +3810,7 @@
         <v>5.6548699999999998</v>
       </c>
       <c r="D91">
-        <v>-0.39774999999999999</v>
+        <v>-0.26976805999999998</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -3824,7 +3824,7 @@
         <v>5.7176999999999998</v>
       </c>
       <c r="D92">
-        <v>-0.28125</v>
+        <v>3.1934104999999997E-2</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -3838,7 +3838,7 @@
         <v>5.7805299999999997</v>
       </c>
       <c r="D93">
-        <v>-0.15826999999999999</v>
+        <v>0.36554414000000002</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -3852,7 +3852,7 @@
         <v>5.8433599999999997</v>
       </c>
       <c r="D94">
-        <v>-2.9239999999999999E-2</v>
+        <v>0.73244363000000001</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -3866,7 +3866,7 @@
         <v>5.9061899999999996</v>
       </c>
       <c r="D95">
-        <v>0.10535</v>
+        <v>1.1340386</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -3880,7 +3880,7 @@
         <v>5.9690300000000001</v>
       </c>
       <c r="D96">
-        <v>0.24503</v>
+        <v>1.5718319999999999</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -3894,7 +3894,7 @@
         <v>6.03186</v>
       </c>
       <c r="D97">
-        <v>0.38923000000000002</v>
+        <v>2.0471393999999998</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -3908,7 +3908,7 @@
         <v>6.0946899999999999</v>
       </c>
       <c r="D98">
-        <v>0.53739999999999999</v>
+        <v>2.5615070000000002</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -3922,7 +3922,7 @@
         <v>6.1575199999999999</v>
       </c>
       <c r="D99">
-        <v>0.68898999999999999</v>
+        <v>3.1164382000000002</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -3936,7 +3936,7 @@
         <v>6.2203499999999998</v>
       </c>
       <c r="D100">
-        <v>0.84338999999999997</v>
+        <v>3.7134610000000001</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3950,7 +3950,7 @@
         <v>6.2831900000000003</v>
       </c>
       <c r="D101">
-        <v>1.0000100000000001</v>
+        <v>4.3542337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>